<commit_message>
All of the Planets
All of the planets have been added with Eccentric Circles and Paths
shown. More correct information is shown in the info window
</commit_message>
<xml_diff>
--- a/PlanetData.xlsx
+++ b/PlanetData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Planets</t>
   </si>
@@ -78,19 +78,22 @@
     <t>Orbital period (s)</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Velocity^2</t>
-  </si>
-  <si>
-    <t>Acceleration</t>
-  </si>
-  <si>
-    <t>Force</t>
+    <t>Eccentricity</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Velocity Km/s</t>
+  </si>
+  <si>
+    <t>Rotation (hours)</t>
+  </si>
+  <si>
+    <t>Earths Moon</t>
+  </si>
+  <si>
+    <t>http://nssdc.gsfc.nasa.gov/planetary/factsheet/moonfact.html</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,9 +452,13 @@
     <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="28.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,8 +489,20 @@
       <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -513,8 +532,11 @@
         <f>2*3.14159*SQRT((I2*I2*I2)/B$14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -544,8 +566,17 @@
         <f t="shared" ref="J3:J10" si="1">2*3.14159*SQRT((I3*I3*I3)/B$14)</f>
         <v>960900877.70378053</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>0.2056</v>
+      </c>
+      <c r="M3">
+        <v>47.4</v>
+      </c>
+      <c r="N3">
+        <v>1407.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -575,8 +606,17 @@
         <f t="shared" si="1"/>
         <v>2441587163.2675638</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="M4">
+        <v>35</v>
+      </c>
+      <c r="N4">
+        <v>-5835.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -606,8 +646,17 @@
         <f t="shared" si="1"/>
         <v>3976476211.5766444</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>1.67E-2</v>
+      </c>
+      <c r="M5">
+        <v>29.8</v>
+      </c>
+      <c r="N5">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -637,8 +686,17 @@
         <f t="shared" si="1"/>
         <v>7440041971.2161713</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="M6">
+        <v>24.1</v>
+      </c>
+      <c r="N6">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -668,8 +726,17 @@
         <f t="shared" si="1"/>
         <v>47298001012.166656</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="M7">
+        <v>13.1</v>
+      </c>
+      <c r="N7">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -699,8 +766,17 @@
         <f t="shared" si="1"/>
         <v>117636110308.8371</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="M8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N8">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -730,8 +806,17 @@
         <f t="shared" si="1"/>
         <v>335346187494.89722</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>4.7199999999999999E-2</v>
+      </c>
+      <c r="M9">
+        <v>6.8</v>
+      </c>
+      <c r="N9">
+        <v>-17.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -761,8 +846,46 @@
         <f t="shared" si="1"/>
         <v>656682390392.29749</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K10">
+        <v>8.6E-3</v>
+      </c>
+      <c r="M10">
+        <v>5.4</v>
+      </c>
+      <c r="N10">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="D12">
+        <v>3.34</v>
+      </c>
+      <c r="E12">
+        <v>1737.5</v>
+      </c>
+      <c r="F12">
+        <v>0.378</v>
+      </c>
+      <c r="G12">
+        <v>0.36330000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="I12">
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="K12">
+        <v>5.4899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -771,101 +894,25 @@
         <v>6.6738400000000001E-11</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19">
-        <v>0.72045356000000005</v>
-      </c>
-      <c r="C19">
-        <f>A19*A19+A20*A20</f>
-        <v>0.51917445781330063</v>
-      </c>
-      <c r="D19">
-        <f>SQRT(C19)</f>
-        <v>0.72053761720905363</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19">
-        <f>D19/214441.8</f>
-        <v>3.3600614115767245E-6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20">
-        <v>1.1005712000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22">
-        <v>8.5195999999999994E-2</v>
-      </c>
-      <c r="C22">
-        <f>A22*A22+A23*A23</f>
-        <v>31.110187358415999</v>
-      </c>
-      <c r="D22" s="2">
-        <f>C22/B24</f>
-        <v>6.7726931417432081E-3</v>
-      </c>
-      <c r="E22" s="2">
-        <f>D22*106</f>
-        <v>0.71790547302478003</v>
-      </c>
-      <c r="F22">
-        <f>SQRT(E22)</f>
-        <v>0.8472930266588885</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23">
-        <v>5.577</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="2">
-        <v>21100000</v>
-      </c>
-      <c r="B24">
-        <f>SQRT(A24)</f>
-        <v>4593.4736311423403</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="E25" s="2">
-        <v>1.469E-6</v>
-      </c>
+    <row r="20" spans="1:7">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="28" spans="1:8">
-      <c r="F28" s="2">
-        <f>D19/D22</f>
-        <v>106.38864069716233</v>
-      </c>
-      <c r="G28" s="2">
-        <f>F28*A24</f>
-        <v>2244800318.710125</v>
-      </c>
-      <c r="H28">
-        <f>SQRT(G28)</f>
-        <v>47379.323746863723</v>
-      </c>
+    <row r="28" spans="1:7">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>